<commit_message>
[SONALI]:Adding final code with report
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel1.xlsx
+++ b/src/test/resources/Excel1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVARKAR\eclipse-workspace\coverfox\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C82644-4C1A-4785-94B0-EFBD4F510089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0606CCCF-9E02-47FB-B35A-0D03CBD59CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{3EA91225-DFB8-4D30-AC02-72B018AA2D1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Hello</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>411028</t>
+  </si>
+  <si>
+    <t>9999999999</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>